<commit_message>
This actually kind of works. Please work.
</commit_message>
<xml_diff>
--- a/uploads/log.xlsx
+++ b/uploads/log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiwi_\Documents\Programming\Forecast\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b71d31f1b3b0162/Smith Tank and Trailer Repair/Tests and Inspections/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF8D254-2C6F-48F1-BDEB-B226987F7480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="541" documentId="13_ncr:1_{65F1E305-C39F-4E19-8DE8-FCC320F4D700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A44FFB5E-203B-4527-92CD-B68625D4E7D3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Control Sheet -August, 2023" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5779" uniqueCount="1054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5759" uniqueCount="1052">
   <si>
     <t xml:space="preserve">WO# </t>
   </si>
@@ -3194,12 +3194,6 @@
   </si>
   <si>
     <t>3S7007</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -3937,8 +3931,8 @@
   <dimension ref="A1:Q73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52:O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6611,56 +6605,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
-        <v>4495</v>
-      </c>
-      <c r="B54" s="70">
-        <v>44941</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L54" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q54" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>1011</v>
@@ -7383,7 +7327,7 @@
   <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+      <selection sqref="A1:I141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11060,10 +11004,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P960"/>
+  <dimension ref="A1:I960"/>
   <sheetViews>
-    <sheetView topLeftCell="A795" workbookViewId="0">
-      <selection activeCell="D781" sqref="D781"/>
+    <sheetView topLeftCell="A745" workbookViewId="0">
+      <selection activeCell="D749" sqref="D749"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35557,7 +35501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="945" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A945" s="10">
         <v>3706</v>
       </c>
@@ -35583,7 +35527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="946" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="946" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A946" s="10">
         <v>4084</v>
       </c>
@@ -35609,7 +35553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="947" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="947" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A947" s="10">
         <v>4190</v>
       </c>
@@ -35635,7 +35579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="948" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="948" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A948" s="10">
         <v>4219</v>
       </c>
@@ -35661,7 +35605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="949" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A949" s="10">
         <v>4222</v>
       </c>
@@ -35686,11 +35630,8 @@
       <c r="I949">
         <v>4</v>
       </c>
-      <c r="P949" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="950" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="950" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A950" s="10">
         <v>4227</v>
       </c>
@@ -35716,7 +35657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="951" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A951" s="10">
         <v>4228</v>
       </c>
@@ -35742,7 +35683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="952" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A952" s="10">
         <v>4241</v>
       </c>
@@ -35768,7 +35709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="953" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="953" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A953" s="10">
         <v>4249</v>
       </c>
@@ -35794,7 +35735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="954" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A954" s="10">
         <v>4256</v>
       </c>
@@ -35820,7 +35761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="955" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="955" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A955" s="10">
         <v>4258</v>
       </c>
@@ -35846,7 +35787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="956" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="956" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A956" s="10">
         <v>4276</v>
       </c>
@@ -35872,7 +35813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="957" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="957" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A957" s="10">
         <v>4278</v>
       </c>
@@ -35898,7 +35839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="958" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="958" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A958" s="10">
         <v>4292</v>
       </c>
@@ -35924,33 +35865,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="959" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A959" s="10" t="s">
-        <v>1052</v>
-      </c>
-      <c r="B959" s="10">
-        <v>307</v>
-      </c>
-      <c r="C959" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D959" s="12" t="s">
-        <v>405</v>
-      </c>
-      <c r="E959" s="13" t="s">
-        <v>659</v>
-      </c>
-      <c r="F959" s="73">
-        <v>45177</v>
-      </c>
-      <c r="G959" s="13" t="s">
-        <v>1008</v>
-      </c>
-      <c r="I959">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="960" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Start of Calendar process. Moveable element works as a starting point
</commit_message>
<xml_diff>
--- a/uploads/log.xlsx
+++ b/uploads/log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b71d31f1b3b0162/Smith Tank and Trailer Repair/Tests and Inspections/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="541" documentId="13_ncr:1_{65F1E305-C39F-4E19-8DE8-FCC320F4D700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A44FFB5E-203B-4527-92CD-B68625D4E7D3}"/>
+  <xr:revisionPtr revIDLastSave="714" documentId="13_ncr:1_{65F1E305-C39F-4E19-8DE8-FCC320F4D700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EE7E273-7B54-48E8-95ED-003E95C4E79C}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5759" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5955" uniqueCount="1066">
   <si>
     <t xml:space="preserve">WO# </t>
   </si>
@@ -3194,6 +3194,48 @@
   </si>
   <si>
     <t>3S7007</t>
+  </si>
+  <si>
+    <t>22524LR</t>
+  </si>
+  <si>
+    <t>44-1449</t>
+  </si>
+  <si>
+    <t>MC DOT 331</t>
+  </si>
+  <si>
+    <t>Matec</t>
+  </si>
+  <si>
+    <t>ME-432</t>
+  </si>
+  <si>
+    <t>TC 406 AL</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>4686</t>
+  </si>
+  <si>
+    <t>4687</t>
+  </si>
+  <si>
+    <t>Jun Chae</t>
+  </si>
+  <si>
+    <t>41-0390</t>
+  </si>
+  <si>
+    <t>Northside Petroleum</t>
+  </si>
+  <si>
+    <t>22525LR</t>
+  </si>
+  <si>
+    <t>1602</t>
   </si>
 </sst>
 </file>
@@ -3403,7 +3445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3611,11 +3653,474 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3625,6 +4130,213 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -3928,11 +4640,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52:O53"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6605,703 +7317,1403 @@
         <v>18</v>
       </c>
     </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
+        <v>4555</v>
+      </c>
+      <c r="B54" s="70">
+        <v>45223</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L54" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q54" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="10">
+        <v>4557</v>
+      </c>
+      <c r="B55" s="70">
+        <v>45224</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q55" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="10">
+        <v>4559</v>
+      </c>
+      <c r="B56" s="70">
+        <v>45224</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>792</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="M56" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="N56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O56" s="10" t="s">
+        <v>1043</v>
+      </c>
+      <c r="Q56" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="10">
+        <v>4565</v>
+      </c>
+      <c r="B57" s="70">
+        <v>45225</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L57" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q57" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="10">
+        <v>4561</v>
+      </c>
+      <c r="B58" s="70">
+        <v>45225</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>554</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L58" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q58" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="10">
+        <v>4562</v>
+      </c>
+      <c r="B59" s="70">
+        <v>45225</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L59" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q59" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="10">
+        <v>4563</v>
+      </c>
+      <c r="B60" s="70">
+        <v>45225</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L60" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O60" s="10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q60" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="10">
+        <v>4564</v>
+      </c>
+      <c r="B61" s="70">
+        <v>45225</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L61" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q61" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="10">
+        <v>4567</v>
+      </c>
+      <c r="B62" s="70">
+        <v>45226</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>1010</v>
+      </c>
+      <c r="M62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O62" s="95" t="s">
+        <v>1043</v>
+      </c>
+      <c r="Q62" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="10">
+        <v>4568</v>
+      </c>
+      <c r="B63" s="70">
+        <v>45226</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>874</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L63" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q63" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="10">
+        <v>4569</v>
+      </c>
+      <c r="B64" s="70">
+        <v>45226</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L64" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q64" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="10">
+        <v>4577</v>
+      </c>
+      <c r="B65" s="70">
+        <v>45229</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L65" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M65" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N65" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O65" s="10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q65" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" s="10">
+        <v>4587</v>
+      </c>
+      <c r="B66" s="70">
+        <v>45231</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>867</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L66" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q66" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" s="10">
+        <v>4591</v>
+      </c>
+      <c r="B67" s="70">
+        <v>45231</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L67" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O67" s="95" t="s">
+        <v>1043</v>
+      </c>
+      <c r="Q67" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B88" s="4">
         <v>45169</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D60" s="63" t="s">
+      <c r="D88" s="63" t="s">
         <v>810</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G60" s="5" t="s">
+      <c r="F88" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L60" s="5" t="s">
+      <c r="H88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L88" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q60" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="M88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q88" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B89" s="4">
         <v>45169</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D61" s="63" t="s">
+      <c r="D89" s="63" t="s">
         <v>539</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>1013</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G61" s="5" t="s">
+      <c r="F89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G89" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L61" s="5" t="s">
+      <c r="H89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L89" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q61" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="M89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q89" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B90" s="4">
         <v>45169</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D62" s="63" t="s">
+      <c r="D90" s="63" t="s">
         <v>540</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>1014</v>
       </c>
-      <c r="F62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G62" s="5" t="s">
+      <c r="F90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L62" s="5" t="s">
+      <c r="H90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L90" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q62" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="M90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q90" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B91" s="4">
         <v>45169</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D63" s="63" t="s">
+      <c r="D91" s="63" t="s">
         <v>1015</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E91" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G63" s="5" t="s">
+      <c r="F91" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G91" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H91" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K63" s="5" t="s">
+      <c r="I91" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K91" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="L63" s="5" t="s">
+      <c r="L91" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M63" s="5" t="s">
+      <c r="M91" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="N63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q63" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="N91" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O91" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q91" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B92" s="4">
         <v>45169</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D64" s="63" t="s">
+      <c r="D92" s="63" t="s">
         <v>1016</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" s="5" t="s">
+      <c r="F92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G92" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H92" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I92" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="J64" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K64" s="5" t="s">
+      <c r="J92" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K92" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="L64" s="5" t="s">
+      <c r="L92" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M64" s="5" t="s">
+      <c r="M92" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="N64" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O64" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q64" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="N92" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O92" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q92" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B93" s="4">
         <v>45169</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="D65" s="63" t="s">
+      <c r="D93" s="63" t="s">
         <v>1017</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G65" s="5" t="s">
+      <c r="F93" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H93" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I65" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K65" s="5" t="s">
+      <c r="I93" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K93" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="L65" s="5" t="s">
+      <c r="L93" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M65" s="5" t="s">
+      <c r="M93" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="N65" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O65" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q65" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="N93" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O93" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q93" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B94" s="4">
         <v>45169</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D66" s="63" t="s">
+      <c r="D94" s="63" t="s">
         <v>1019</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>1020</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H66" s="5" t="s">
+      <c r="F94" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H94" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q66" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="I94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q94" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B95" s="4">
         <v>45169</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D67" s="63" t="s">
+      <c r="D95" s="63" t="s">
         <v>1021</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G67" s="5" t="s">
+      <c r="F95" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G95" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H67" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K67" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L67" s="5" t="s">
+      <c r="H95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L95" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M67" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N67" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O67" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q67" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="M95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q95" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B96" s="4">
         <v>45169</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D68" s="63" t="s">
+      <c r="D96" s="63" t="s">
         <v>405</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G68" s="5" t="s">
+      <c r="F96" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G96" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H96" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K68" s="5" t="s">
+      <c r="I96" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K96" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="L68" s="5" t="s">
+      <c r="L96" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M68" s="5" t="s">
+      <c r="M96" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="N68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q68" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="N96" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O96" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q96" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B97" s="4">
         <v>45169</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D69" s="63" t="s">
+      <c r="D97" s="63" t="s">
         <v>1022</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G69" s="5" t="s">
+      <c r="F97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G97" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L69" s="5" t="s">
+      <c r="H97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L97" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q69" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="M97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O97" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q97" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B98" s="4">
         <v>45169</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D70" s="63" t="s">
+      <c r="D98" s="63" t="s">
         <v>1023</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>1024</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G70" s="5" t="s">
+      <c r="F98" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G98" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L70" s="5" t="s">
+      <c r="H98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L98" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q70" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="M98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q98" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B99" s="4">
         <v>45169</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D71" s="63">
+      <c r="D99" s="63">
         <v>135725</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E99" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" s="5" t="s">
+      <c r="F99" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G99" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L71" s="5" t="s">
+      <c r="H99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L99" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q71" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="M99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O99" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q99" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B100" s="4">
         <v>45169</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D72" s="63" t="s">
+      <c r="D100" s="63" t="s">
         <v>1025</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G72" s="5" t="s">
+      <c r="F100" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G100" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H100" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I72" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K72" s="5" t="s">
+      <c r="I100" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K100" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="L72" s="5" t="s">
+      <c r="L100" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M72" s="5" t="s">
+      <c r="M100" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="N72" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O72" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q72" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="N100" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O100" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q100" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B101" s="4">
         <v>45169</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C101" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="D73" s="63" t="s">
+      <c r="D101" s="63" t="s">
         <v>504</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G73" s="5" t="s">
+      <c r="F101" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G101" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H101" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="I73" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K73" s="5" t="s">
+      <c r="I101" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K101" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="L73" s="5" t="s">
+      <c r="L101" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="M73" s="5" t="s">
+      <c r="M101" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="N73" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O73" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q73" s="5" t="s">
+      <c r="N101" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O101" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q101" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -7309,9 +8721,154 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:XFD23">
     <sortCondition ref="A3:A23"/>
   </sortState>
-  <conditionalFormatting sqref="A1:Q1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N/A">
+  <conditionalFormatting sqref="A1:Q55 A56:C56 E56:Q56 A57:Q58 A59:E59 G59:Q59 A78:Q1048576 F59:F61 O62">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60:K60">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M60:O60">
+    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q60">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61:K61">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M61:O61">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q61">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63:K63">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M63:O63">
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q63">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M62:N62">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62:K62">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F62:F63">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",F62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q62">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64:K64">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F64">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",F64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M64:O64">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q64">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O65">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",O65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65:K65">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M65:N65">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q65">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66:K66">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M66:O66">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q66">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O67">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",O67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M67:N67">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67:K67">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",H67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F65:F67">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",F65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q67">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10992,7 +12549,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="91" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
System looks good, happy with where it is at. No more trailing LR or AB, dashes changed to slashes. Calendar needs heavy styling
</commit_message>
<xml_diff>
--- a/uploads/log.xlsx
+++ b/uploads/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b71d31f1b3b0162/Smith Tank and Trailer Repair/Tests and Inspections/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="13_ncr:1_{E869FC2D-C3B1-4EA1-A8B4-086511A1DB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7723E621-2131-40DF-B6D3-FD9E7C195345}"/>
+  <xr:revisionPtr revIDLastSave="304" documentId="13_ncr:1_{E869FC2D-C3B1-4EA1-A8B4-086511A1DB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9176942-A890-419C-8D34-200B00B32598}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Control Sheet -August, 2023" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6124" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6192" uniqueCount="1083">
   <si>
     <t xml:space="preserve">WO# </t>
   </si>
@@ -2943,9 +2943,6 @@
     <t>Paul &amp; Dax</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>237AB</t>
   </si>
   <si>
@@ -3277,6 +3274,21 @@
   </si>
   <si>
     <t>142</t>
+  </si>
+  <si>
+    <t>Signature Flight Support</t>
+  </si>
+  <si>
+    <t>506343</t>
+  </si>
+  <si>
+    <t>440753</t>
+  </si>
+  <si>
+    <t>22828LR</t>
+  </si>
+  <si>
+    <t>Alex Pawliuk (OJT)</t>
   </si>
 </sst>
 </file>
@@ -3722,7 +3734,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3793,14 +3815,119 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -4497,9 +4624,9 @@
   </sheetPr>
   <dimension ref="A1:U110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S79" sqref="A79:S79"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S84" sqref="S84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8482,18 +8609,14 @@
       <c r="E75" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="F75" s="95" t="s">
-        <v>22</v>
-      </c>
+      <c r="F75" s="10"/>
       <c r="G75" s="95" t="s">
         <v>55</v>
       </c>
       <c r="H75" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="I75" s="95" t="s">
-        <v>22</v>
-      </c>
+      <c r="I75" s="10"/>
       <c r="J75" s="95" t="s">
         <v>22</v>
       </c>
@@ -8547,6 +8670,7 @@
       </c>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
       <c r="I76" s="10"/>
       <c r="J76" s="10" t="s">
         <v>22</v>
@@ -8601,6 +8725,7 @@
       </c>
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
       <c r="I77" s="10"/>
       <c r="J77" s="10" t="s">
         <v>22</v>
@@ -8655,6 +8780,7 @@
       </c>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
       <c r="I78" s="10"/>
       <c r="J78" s="10" t="s">
         <v>22</v>
@@ -8699,16 +8825,17 @@
         <v>45250</v>
       </c>
       <c r="C79" s="10" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D79" s="12" t="s">
         <v>1077</v>
-      </c>
-      <c r="D79" s="12" t="s">
-        <v>1078</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
       <c r="I79" s="10"/>
       <c r="J79" s="10" t="s">
         <v>22</v>
@@ -8745,7 +8872,276 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H80" s="35"/>
+      <c r="A80" s="10">
+        <v>4655</v>
+      </c>
+      <c r="B80" s="70">
+        <v>45252</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I80" s="10"/>
+      <c r="J80" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K80" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L80" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M80" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N80" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O80" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P80" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q80" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="R80" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S80" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U80" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A81" s="10">
+        <v>4669</v>
+      </c>
+      <c r="B81" s="70">
+        <v>45254</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K81" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L81" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M81" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N81" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O81" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P81" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q81" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R81" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S81" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U81" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
+        <v>4600</v>
+      </c>
+      <c r="B82" s="70">
+        <v>45257</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>943</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K82" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L82" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M82" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N82" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O82" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P82" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q82" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="R82" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S82" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U82" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A83" s="10">
+        <v>4674</v>
+      </c>
+      <c r="B83" s="70">
+        <v>45258</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K83" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L83" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M83" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N83" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O83" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P83" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q83" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R83" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S83" s="10" t="s">
+        <v>1082</v>
+      </c>
+      <c r="U83" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A84" s="10">
+        <v>4681</v>
+      </c>
+      <c r="B84" s="70">
+        <v>45259</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>952</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P84" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S84" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U84" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H85" s="35"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
@@ -9494,108 +9890,133 @@
     <sortCondition ref="A3:A23"/>
   </sortState>
   <conditionalFormatting sqref="A1:U70 A97:U1048576">
-    <cfRule type="containsText" dxfId="21" priority="37" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="26" priority="59" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F75">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",F75)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I75:J75">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",I75)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J71:J73">
-    <cfRule type="containsText" dxfId="18" priority="33" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="25" priority="55" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",J71)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J77:J78">
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="N/A">
+  <conditionalFormatting sqref="J75">
+    <cfRule type="containsText" dxfId="24" priority="41" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",J75)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:J82">
+    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",J77)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J84">
+    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",J84)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L71:O72">
-    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="21" priority="54" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",L71)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76:O78">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="N/A">
+  <conditionalFormatting sqref="L76:O79">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",L76)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L83:O84">
+    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",L83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M74:M75">
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="18" priority="38" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",M74)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M80:O80">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",M80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N75">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="16" priority="37" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",N75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N73:O73">
-    <cfRule type="containsText" dxfId="12" priority="29" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="15" priority="51" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",N73)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N81:O82">
+    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",N81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O74">
-    <cfRule type="containsText" dxfId="11" priority="25" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="13" priority="47" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",O74)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Q81">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q74:R74">
-    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="11" priority="45" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",Q74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q76:R76">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="10" priority="34" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",Q76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q71:S72">
-    <cfRule type="containsText" dxfId="8" priority="31" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="9" priority="53" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",Q71)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q77:S78">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="N/A">
+  <conditionalFormatting sqref="Q77:S79">
+    <cfRule type="containsText" dxfId="8" priority="25" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",Q77)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Q83:S84">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",Q83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R75:S75">
-    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="6" priority="36" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",R75)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R80:S80">
+    <cfRule type="containsText" dxfId="5" priority="21" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",R80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R82:S82">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",R82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S73:S74">
-    <cfRule type="containsText" dxfId="5" priority="22" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="3" priority="44" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",S73)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U71:U79">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",U71)))</formula>
+  <conditionalFormatting sqref="S81">
+    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",S81)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q79:S79">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",Q79)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L79:O79">
+  <conditionalFormatting sqref="U71:U84">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",L79)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J79">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",J79)))</formula>
+      <formula>NOT(ISERROR(SEARCH("N/A",U71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13317,7 +13738,7 @@
     <mergeCell ref="J1:M9"/>
   </mergeCells>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -13331,8 +13752,8 @@
   </sheetPr>
   <dimension ref="A1:I960"/>
   <sheetViews>
-    <sheetView topLeftCell="A908" workbookViewId="0">
-      <selection activeCell="F500" sqref="F500"/>
+    <sheetView tabSelected="1" topLeftCell="A753" workbookViewId="0">
+      <selection activeCell="I767" sqref="A767:I767"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33211,7 +33632,7 @@
         <v>158</v>
       </c>
       <c r="F767" s="73">
-        <v>45288</v>
+        <v>44923</v>
       </c>
       <c r="G767" s="13" t="s">
         <v>966</v>
@@ -33248,8 +33669,8 @@
       </c>
     </row>
     <row r="769" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A769" s="10" t="s">
-        <v>967</v>
+      <c r="A769" s="10">
+        <v>3382</v>
       </c>
       <c r="B769" s="10">
         <v>331</v>
@@ -33284,7 +33705,7 @@
         <v>59</v>
       </c>
       <c r="D770" s="12" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E770" s="13" t="s">
         <v>158</v>
@@ -33336,7 +33757,7 @@
         <v>39</v>
       </c>
       <c r="D772" s="12" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E772" s="13" t="s">
         <v>158</v>
@@ -33362,7 +33783,7 @@
         <v>702</v>
       </c>
       <c r="D773" s="12" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="E773" s="13" t="s">
         <v>158</v>
@@ -33414,7 +33835,7 @@
         <v>59</v>
       </c>
       <c r="D775" s="12" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E775" s="13" t="s">
         <v>158</v>
@@ -33437,13 +33858,13 @@
         <v>338</v>
       </c>
       <c r="C776" s="11" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D776" s="12" t="s">
         <v>74</v>
       </c>
       <c r="E776" s="13" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F776" s="90">
         <v>44939</v>
@@ -33466,7 +33887,7 @@
         <v>36</v>
       </c>
       <c r="D777" s="12" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="E777" s="13" t="s">
         <v>158</v>
@@ -33518,7 +33939,7 @@
         <v>39</v>
       </c>
       <c r="D779" s="12" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="E779" s="13" t="s">
         <v>158</v>
@@ -33544,7 +33965,7 @@
         <v>59</v>
       </c>
       <c r="D780" s="12" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="E780" s="13" t="s">
         <v>446</v>
@@ -33553,7 +33974,7 @@
         <v>44949</v>
       </c>
       <c r="G780" s="13" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I780">
         <v>1</v>
@@ -33579,7 +34000,7 @@
         <v>44950</v>
       </c>
       <c r="G781" s="13" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I781">
         <v>1</v>
@@ -33596,7 +34017,7 @@
         <v>327</v>
       </c>
       <c r="D782" s="12" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E782" s="13" t="s">
         <v>158</v>
@@ -33645,10 +34066,10 @@
         <v>406</v>
       </c>
       <c r="C784" s="11" t="s">
+        <v>979</v>
+      </c>
+      <c r="D784" s="12" t="s">
         <v>980</v>
-      </c>
-      <c r="D784" s="12" t="s">
-        <v>981</v>
       </c>
       <c r="E784" s="13" t="s">
         <v>446</v>
@@ -33671,7 +34092,7 @@
         <v>407</v>
       </c>
       <c r="C785" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D785" s="12" t="s">
         <v>716</v>
@@ -33726,7 +34147,7 @@
         <v>70</v>
       </c>
       <c r="D787" s="12" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E787" s="13" t="s">
         <v>158</v>
@@ -33749,7 +34170,7 @@
         <v>407</v>
       </c>
       <c r="C788" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D788" s="12" t="s">
         <v>704</v>
@@ -33778,7 +34199,7 @@
         <v>39</v>
       </c>
       <c r="D789" s="12" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E789" s="13" t="s">
         <v>446</v>
@@ -33856,7 +34277,7 @@
         <v>25</v>
       </c>
       <c r="D792" s="12" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E792" s="13" t="s">
         <v>463</v>
@@ -33882,7 +34303,7 @@
         <v>108</v>
       </c>
       <c r="D793" s="12" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E793" s="13" t="s">
         <v>158</v>
@@ -33908,7 +34329,7 @@
         <v>20</v>
       </c>
       <c r="D794" s="12" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E794" s="13" t="s">
         <v>158</v>
@@ -33934,7 +34355,7 @@
         <v>59</v>
       </c>
       <c r="D795" s="12" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E795" s="13" t="s">
         <v>158</v>
@@ -33960,7 +34381,7 @@
         <v>772</v>
       </c>
       <c r="D796" s="12" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E796" s="13" t="s">
         <v>158</v>
@@ -34035,10 +34456,10 @@
         <v>406</v>
       </c>
       <c r="C799" s="11" t="s">
+        <v>989</v>
+      </c>
+      <c r="D799" s="12" t="s">
         <v>990</v>
-      </c>
-      <c r="D799" s="12" t="s">
-        <v>991</v>
       </c>
       <c r="E799" s="13" t="s">
         <v>158</v>
@@ -34064,7 +34485,7 @@
         <v>772</v>
       </c>
       <c r="D800" s="12" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E800" s="13" t="s">
         <v>158</v>
@@ -34090,7 +34511,7 @@
         <v>772</v>
       </c>
       <c r="D801" s="12" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E801" s="13" t="s">
         <v>158</v>
@@ -34116,7 +34537,7 @@
         <v>29</v>
       </c>
       <c r="D802" s="12" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="E802" s="13" t="s">
         <v>463</v>
@@ -34168,7 +34589,7 @@
         <v>59</v>
       </c>
       <c r="D804" s="12" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E804" s="13" t="s">
         <v>158</v>
@@ -34194,7 +34615,7 @@
         <v>59</v>
       </c>
       <c r="D805" s="12" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E805" s="13" t="s">
         <v>158</v>
@@ -34220,7 +34641,7 @@
         <v>39</v>
       </c>
       <c r="D806" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E806" s="13" t="s">
         <v>446</v>
@@ -34273,7 +34694,7 @@
         <v>25</v>
       </c>
       <c r="D808" s="12" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="E808" s="13" t="s">
         <v>941</v>
@@ -34351,7 +34772,7 @@
         <v>102</v>
       </c>
       <c r="D811" s="12" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E811" s="13" t="s">
         <v>158</v>
@@ -34455,7 +34876,7 @@
         <v>39</v>
       </c>
       <c r="D815" s="12" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E815" s="13" t="s">
         <v>158</v>
@@ -34507,7 +34928,7 @@
         <v>20</v>
       </c>
       <c r="D817" s="12" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E817" s="13" t="s">
         <v>466</v>
@@ -34533,7 +34954,7 @@
         <v>59</v>
       </c>
       <c r="D818" s="12" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E818" s="13" t="s">
         <v>446</v>
@@ -34559,7 +34980,7 @@
         <v>39</v>
       </c>
       <c r="D819" s="12" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E819" s="13" t="s">
         <v>158</v>
@@ -34582,10 +35003,10 @@
         <v>306</v>
       </c>
       <c r="C820" s="11" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D820" s="12" t="s">
         <v>1004</v>
-      </c>
-      <c r="D820" s="12" t="s">
-        <v>1005</v>
       </c>
       <c r="E820" s="13" t="s">
         <v>158</v>
@@ -34634,10 +35055,10 @@
         <v>331</v>
       </c>
       <c r="C822" s="11" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D822" s="12" t="s">
         <v>1006</v>
-      </c>
-      <c r="D822" s="12" t="s">
-        <v>1007</v>
       </c>
       <c r="E822" s="13" t="s">
         <v>158</v>
@@ -34767,7 +35188,7 @@
         <v>39</v>
       </c>
       <c r="D827" s="12" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E827" s="13" t="s">
         <v>158</v>
@@ -34819,7 +35240,7 @@
         <v>29</v>
       </c>
       <c r="D829" s="12" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="E829" s="13" t="s">
         <v>158</v>
@@ -34845,7 +35266,7 @@
         <v>39</v>
       </c>
       <c r="D830" s="12" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="E830" s="13" t="s">
         <v>158</v>
@@ -34923,7 +35344,7 @@
         <v>59</v>
       </c>
       <c r="D833" s="12" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E833" s="13" t="s">
         <v>158</v>
@@ -34949,7 +35370,7 @@
         <v>772</v>
       </c>
       <c r="D834" s="12" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E834" s="13" t="s">
         <v>158</v>
@@ -35001,7 +35422,7 @@
         <v>39</v>
       </c>
       <c r="D836" s="12" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E836" s="13" t="s">
         <v>158</v>
@@ -35079,7 +35500,7 @@
         <v>59</v>
       </c>
       <c r="D839" s="12" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="E839" s="13" t="s">
         <v>446</v>
@@ -35105,10 +35526,10 @@
         <v>172</v>
       </c>
       <c r="D840" s="12" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E840" s="13" t="s">
         <v>1015</v>
-      </c>
-      <c r="E840" s="13" t="s">
-        <v>1016</v>
       </c>
       <c r="F840" s="90">
         <v>45017</v>
@@ -35128,10 +35549,10 @@
         <v>406</v>
       </c>
       <c r="C841" s="11" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D841" s="12" t="s">
         <v>1017</v>
-      </c>
-      <c r="D841" s="12" t="s">
-        <v>1018</v>
       </c>
       <c r="E841" s="13" t="s">
         <v>158</v>
@@ -35140,7 +35561,7 @@
         <v>45017</v>
       </c>
       <c r="G841" s="13" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I841">
         <v>2</v>
@@ -35160,7 +35581,7 @@
         <v>282</v>
       </c>
       <c r="E842" s="13" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F842" s="90">
         <v>45019</v>
@@ -35180,7 +35601,7 @@
         <v>306</v>
       </c>
       <c r="C843" s="11" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D843" s="12" t="s">
         <v>760</v>
@@ -35232,7 +35653,7 @@
         <v>331</v>
       </c>
       <c r="C845" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D845" s="12" t="s">
         <v>808</v>
@@ -35261,7 +35682,7 @@
         <v>39</v>
       </c>
       <c r="D846" s="12" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="E846" s="13" t="s">
         <v>446</v>
@@ -35336,7 +35757,7 @@
         <v>407</v>
       </c>
       <c r="C849" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D849" s="12" t="s">
         <v>803</v>
@@ -35374,7 +35795,7 @@
         <v>45026</v>
       </c>
       <c r="G850" s="13" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I850">
         <v>2</v>
@@ -35414,10 +35835,10 @@
         <v>406</v>
       </c>
       <c r="C852" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D852" s="12" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="E852" s="13" t="s">
         <v>158</v>
@@ -35470,7 +35891,7 @@
         <v>59</v>
       </c>
       <c r="D854" s="12" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E854" s="13" t="s">
         <v>158</v>
@@ -35522,7 +35943,7 @@
         <v>59</v>
       </c>
       <c r="D856" s="12" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="E856" s="13" t="s">
         <v>158</v>
@@ -35548,7 +35969,7 @@
         <v>39</v>
       </c>
       <c r="D857" s="12" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E857" s="13" t="s">
         <v>158</v>
@@ -35574,7 +35995,7 @@
         <v>39</v>
       </c>
       <c r="D858" s="12" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E858" s="13" t="s">
         <v>158</v>
@@ -35600,7 +36021,7 @@
         <v>59</v>
       </c>
       <c r="D859" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E859" s="13" t="s">
         <v>325</v>
@@ -35652,7 +36073,7 @@
         <v>25</v>
       </c>
       <c r="D861" s="12" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E861" s="13" t="s">
         <v>283</v>
@@ -35704,7 +36125,7 @@
         <v>56</v>
       </c>
       <c r="D863" s="12" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E863" s="13" t="s">
         <v>158</v>
@@ -35730,7 +36151,7 @@
         <v>56</v>
       </c>
       <c r="D864" s="12" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E864" s="13" t="s">
         <v>158</v>
@@ -35808,7 +36229,7 @@
         <v>39</v>
       </c>
       <c r="D867" s="12" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E867" s="13" t="s">
         <v>158</v>
@@ -35912,7 +36333,7 @@
         <v>39</v>
       </c>
       <c r="D871" s="12" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E871" s="13" t="s">
         <v>158</v>
@@ -35961,10 +36382,10 @@
         <v>406</v>
       </c>
       <c r="C873" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D873" s="12" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="E873" s="13" t="s">
         <v>158</v>
@@ -35990,7 +36411,7 @@
         <v>47</v>
       </c>
       <c r="D874" s="12" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E874" s="13" t="s">
         <v>158</v>
@@ -36094,7 +36515,7 @@
         <v>56</v>
       </c>
       <c r="D878" s="12" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E878" s="13" t="s">
         <v>466</v>
@@ -36117,13 +36538,13 @@
         <v>407</v>
       </c>
       <c r="C879" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D879" s="12" t="s">
         <v>265</v>
       </c>
       <c r="E879" s="13" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F879" s="73">
         <v>45043</v>
@@ -36146,7 +36567,7 @@
         <v>25</v>
       </c>
       <c r="D880" s="12" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E880" s="13" t="s">
         <v>158</v>
@@ -36172,7 +36593,7 @@
         <v>25</v>
       </c>
       <c r="D881" s="12" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E881" s="13" t="s">
         <v>734</v>
@@ -36224,7 +36645,7 @@
         <v>36</v>
       </c>
       <c r="D883" s="12" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E883" s="13" t="s">
         <v>158</v>
@@ -36302,7 +36723,7 @@
         <v>118</v>
       </c>
       <c r="D886" s="12" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E886" s="13" t="s">
         <v>158</v>
@@ -36325,10 +36746,10 @@
         <v>406</v>
       </c>
       <c r="C887" s="11" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D887" s="12" t="s">
         <v>1042</v>
-      </c>
-      <c r="D887" s="12" t="s">
-        <v>1043</v>
       </c>
       <c r="E887" s="13" t="s">
         <v>158</v>
@@ -36377,10 +36798,10 @@
         <v>306</v>
       </c>
       <c r="C889" s="11" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D889" s="12" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E889" s="13" t="s">
         <v>158</v>
@@ -36389,7 +36810,7 @@
         <v>45057</v>
       </c>
       <c r="G889" s="13" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I889">
         <v>3</v>
@@ -36415,7 +36836,7 @@
         <v>45057</v>
       </c>
       <c r="G890" s="13" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I890">
         <v>3</v>
@@ -36559,7 +36980,7 @@
         <v>331</v>
       </c>
       <c r="C896" s="11" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D896" s="12" t="s">
         <v>170</v>
@@ -36571,7 +36992,7 @@
         <v>45064</v>
       </c>
       <c r="G896" s="13" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I896">
         <v>3</v>
@@ -36611,7 +37032,7 @@
         <v>412</v>
       </c>
       <c r="C898" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D898" s="12" t="s">
         <v>900</v>
@@ -36640,7 +37061,7 @@
         <v>59</v>
       </c>
       <c r="D899" s="12" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E899" s="13" t="s">
         <v>158</v>
@@ -36718,7 +37139,7 @@
         <v>20</v>
       </c>
       <c r="D902" s="12" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E902" s="13" t="s">
         <v>158</v>
@@ -36767,7 +37188,7 @@
         <v>407</v>
       </c>
       <c r="C904" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D904" s="12" t="s">
         <v>887</v>
@@ -36793,10 +37214,10 @@
         <v>407</v>
       </c>
       <c r="C905" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D905" s="12" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E905" s="13" t="s">
         <v>941</v>
@@ -36848,7 +37269,7 @@
         <v>59</v>
       </c>
       <c r="D907" s="12" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E907" s="13" t="s">
         <v>158</v>
@@ -36871,7 +37292,7 @@
         <v>417</v>
       </c>
       <c r="C908" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D908" s="12" t="s">
         <v>409</v>
@@ -37014,7 +37435,7 @@
         <v>45089</v>
       </c>
       <c r="G913" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="I913">
         <v>4</v>
@@ -37025,7 +37446,7 @@
         <v>4079</v>
       </c>
       <c r="B914" s="10" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C914" s="11" t="s">
         <v>828</v>
@@ -37057,7 +37478,7 @@
         <v>39</v>
       </c>
       <c r="D915" s="12" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E915" s="13" t="s">
         <v>158</v>
@@ -37066,7 +37487,7 @@
         <v>45090</v>
       </c>
       <c r="G915" s="13" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="I915">
         <v>4</v>
@@ -37092,7 +37513,7 @@
         <v>45091</v>
       </c>
       <c r="G916" s="13" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="I916">
         <v>4</v>
@@ -37118,7 +37539,7 @@
         <v>45092</v>
       </c>
       <c r="G917" s="13" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="I917">
         <v>4</v>
@@ -37135,7 +37556,7 @@
         <v>39</v>
       </c>
       <c r="D918" s="12" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E918" s="13" t="s">
         <v>158</v>
@@ -37144,7 +37565,7 @@
         <v>45093</v>
       </c>
       <c r="G918" s="13" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="I918">
         <v>4</v>
@@ -37161,7 +37582,7 @@
         <v>36</v>
       </c>
       <c r="D919" s="12" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E919" s="13" t="s">
         <v>158</v>
@@ -37213,7 +37634,7 @@
         <v>36</v>
       </c>
       <c r="D921" s="12" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E921" s="13" t="s">
         <v>158</v>
@@ -37222,7 +37643,7 @@
         <v>45100</v>
       </c>
       <c r="G921" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="I921">
         <v>4</v>
@@ -37236,10 +37657,10 @@
         <v>406</v>
       </c>
       <c r="C922" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D922" s="12" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E922" s="13" t="s">
         <v>466</v>
@@ -37268,13 +37689,13 @@
         <v>462</v>
       </c>
       <c r="E923" s="13" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F923" s="73">
         <v>45100</v>
       </c>
       <c r="G923" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="I923">
         <v>4</v>
@@ -37288,10 +37709,10 @@
         <v>406</v>
       </c>
       <c r="C924" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D924" s="12" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E924" s="13" t="s">
         <v>158</v>
@@ -37395,7 +37816,7 @@
         <v>39</v>
       </c>
       <c r="D928" s="12" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E928" s="13" t="s">
         <v>158</v>
@@ -37418,10 +37839,10 @@
         <v>406</v>
       </c>
       <c r="C929" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D929" s="12" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E929" s="13" t="s">
         <v>158</v>
@@ -37430,7 +37851,7 @@
         <v>45106</v>
       </c>
       <c r="G929" s="13" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="I929">
         <v>4</v>
@@ -37444,7 +37865,7 @@
         <v>407</v>
       </c>
       <c r="C930" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D930" s="12" t="s">
         <v>390</v>
@@ -37499,7 +37920,7 @@
         <v>39</v>
       </c>
       <c r="D932" s="12" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E932" s="13" t="s">
         <v>446</v>
@@ -37522,10 +37943,10 @@
         <v>331</v>
       </c>
       <c r="C933" s="11" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D933" s="12" t="s">
         <v>1006</v>
-      </c>
-      <c r="D933" s="12" t="s">
-        <v>1007</v>
       </c>
       <c r="E933" s="13" t="s">
         <v>403</v>
@@ -37551,7 +37972,7 @@
         <v>36</v>
       </c>
       <c r="D934" s="12" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E934" s="13" t="s">
         <v>158</v>
@@ -37577,7 +37998,7 @@
         <v>828</v>
       </c>
       <c r="D935" s="12" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E935" s="13" t="s">
         <v>302</v>
@@ -37603,7 +38024,7 @@
         <v>39</v>
       </c>
       <c r="D936" s="12" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E936" s="13" t="s">
         <v>158</v>
@@ -37629,7 +38050,7 @@
         <v>36</v>
       </c>
       <c r="D937" s="12" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E937" s="13" t="s">
         <v>158</v>
@@ -37785,7 +38206,7 @@
         <v>47</v>
       </c>
       <c r="D943" s="12" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E943" s="13" t="s">
         <v>158</v>
@@ -37915,7 +38336,7 @@
         <v>102</v>
       </c>
       <c r="D948" s="12" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E948" s="13" t="s">
         <v>158</v>
@@ -37967,7 +38388,7 @@
         <v>102</v>
       </c>
       <c r="D950" s="12" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E950" s="13" t="s">
         <v>158</v>
@@ -37976,7 +38397,7 @@
         <v>45125</v>
       </c>
       <c r="G950" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="I950">
         <v>4</v>
@@ -38002,7 +38423,7 @@
         <v>45126</v>
       </c>
       <c r="G951" s="13" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="I951">
         <v>4</v>
@@ -38045,7 +38466,7 @@
         <v>29</v>
       </c>
       <c r="D953" s="12" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E953" s="13" t="s">
         <v>941</v>
@@ -38094,7 +38515,7 @@
         <v>407</v>
       </c>
       <c r="C955" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D955" s="12" t="s">
         <v>903</v>
@@ -38123,7 +38544,7 @@
         <v>39</v>
       </c>
       <c r="D956" s="12" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E956" s="13" t="s">
         <v>158</v>
@@ -38132,7 +38553,7 @@
         <v>45139</v>
       </c>
       <c r="G956" s="13" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="I956">
         <v>4</v>
@@ -38158,7 +38579,7 @@
         <v>45141</v>
       </c>
       <c r="G957" s="13" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="I957">
         <v>4</v>
@@ -38184,7 +38605,7 @@
         <v>45146</v>
       </c>
       <c r="G958" s="13" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="I958">
         <v>4</v>

</xml_diff>